<commit_message>
Added AddIntoExcelFile task from ADO.NET homework
</commit_message>
<xml_diff>
--- a/Software-Technologies/Databases/06.ADO.NET/ReadFromExcelFile/input.xlsx
+++ b/Software-Technologies/Databases/06.ADO.NET/ReadFromExcelFile/input.xlsx
@@ -61,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -69,13 +69,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,41 +402,45 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>33</v>
       </c>
     </row>

</xml_diff>